<commit_message>
revert to sprint-II checklist analysis try
</commit_message>
<xml_diff>
--- a/server/temp/checklist_test.xlsx
+++ b/server/temp/checklist_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="42">
   <si>
     <t>English Name</t>
   </si>
@@ -140,18 +140,6 @@
   </si>
   <si>
     <t>Tandin Wangchuk44256-1</t>
-  </si>
-  <si>
-    <t>Tshering Dorji</t>
-  </si>
-  <si>
-    <t>Tshering Dorji44256-1</t>
-  </si>
-  <si>
-    <t>Tshering Norbu</t>
-  </si>
-  <si>
-    <t>Tshering Norbu44256-1</t>
   </si>
 </sst>
 </file>
@@ -160,9 +148,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="24">
@@ -199,6 +187,44 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -206,13 +232,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -221,39 +256,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -267,33 +270,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -306,38 +295,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,61 +346,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -424,121 +514,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,11 +612,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -651,23 +645,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -683,6 +662,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -726,148 +714,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1222,15 +1210,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="18.6666666666667" customWidth="1"/>
+    <col min="5" max="5" width="11.4444444444444"/>
     <col min="9" max="9" width="17.1111111111111" customWidth="1"/>
     <col min="10" max="10" width="28.2222222222222" customWidth="1"/>
     <col min="11" max="11" width="23.8888888888889" customWidth="1"/>
@@ -1896,93 +1885,6 @@
         <v>41</v>
       </c>
       <c r="K23" s="10"/>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11">
-        <v>5</v>
-      </c>
-      <c r="E24" s="12">
-        <v>44199</v>
-      </c>
-      <c r="F24" s="13">
-        <v>0.417719907407407</v>
-      </c>
-      <c r="G24" s="11">
-        <v>27.20978</v>
-      </c>
-      <c r="H24" s="11">
-        <v>90.06545</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="K24" s="10"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11">
-        <v>5</v>
-      </c>
-      <c r="E25" s="12">
-        <v>44199</v>
-      </c>
-      <c r="F25" s="13">
-        <v>0.737615740740741</v>
-      </c>
-      <c r="G25" s="11">
-        <v>26.96533</v>
-      </c>
-      <c r="H25" s="11">
-        <v>90.86305</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K25" s="10"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="11">
-        <v>5</v>
-      </c>
-      <c r="E26" s="12">
-        <v>44199</v>
-      </c>
-      <c r="F26" s="13">
-        <v>0.317488425925926</v>
-      </c>
-      <c r="G26" s="11">
-        <v>26.75694</v>
-      </c>
-      <c r="H26" s="11">
-        <v>90.13804</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>